<commit_message>
29-9-25 : First Commit
</commit_message>
<xml_diff>
--- a/Documents/MARK MODULE.xlsx
+++ b/Documents/MARK MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DotPinMakrerFrameWrok\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A07DB27-B8C1-4616-A1E1-42DD2EA1E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CBD2A-8EE1-4229-A2D4-4F24EEF6E1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6A3B55C-2917-40CD-AAE1-C5ACFAB4A370}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="486">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -2119,7 +2119,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2141,6 +2141,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2172,7 +2184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2185,17 +2197,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2205,6 +2211,32 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2521,10 +2553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7B9B8E-6A40-4E67-8E1B-E77849CC5C8E}">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2545,7 +2577,7 @@
     <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2586,618 +2618,636 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="72">
-      <c r="A3" s="3" t="s">
+      <c r="L2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="15">
+        <v>1</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="12" customFormat="1" ht="72">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="72">
-      <c r="A4" s="3" t="s">
+      <c r="L3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="15">
+        <v>1</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="12" customFormat="1" ht="72">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="57.6">
-      <c r="A5" s="3" t="s">
+      <c r="L4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="15">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="12" customFormat="1" ht="57.6">
+      <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="J5" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="86.4">
-      <c r="A6" s="3" t="s">
+      <c r="L5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="15">
+        <v>1</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="12" customFormat="1" ht="86.4">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="J6" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="43.2">
-      <c r="A7" s="3" t="s">
+      <c r="L6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="43.2">
-      <c r="A8" s="3" t="s">
+      <c r="L7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="15">
+        <v>1</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="J8" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="43.2">
-      <c r="A9" s="3" t="s">
+      <c r="L8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="43.2">
-      <c r="A10" s="3" t="s">
+      <c r="L9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="J10" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="57.6">
-      <c r="A11" s="3" t="s">
+      <c r="L10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="12" customFormat="1" ht="57.6">
+      <c r="A11" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="J11" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="43.2">
-      <c r="A12" s="3" t="s">
+      <c r="L11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="J12" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="43.2">
-      <c r="A13" s="3" t="s">
+      <c r="L12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="12" customFormat="1" ht="43.2">
+      <c r="A13" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K13" s="3" t="s">
+      <c r="J13" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="57.6">
-      <c r="A14" s="3" t="s">
+      <c r="L13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="12" customFormat="1" ht="57.6">
+      <c r="A14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K14" s="3" t="s">
+      <c r="J14" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="57.6">
-      <c r="A15" s="3" t="s">
+      <c r="L14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="12" customFormat="1" ht="57.6">
+      <c r="A15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="J15" s="14">
+        <v>45923</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="57.6">
-      <c r="A16" s="3" t="s">
+      <c r="L15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="17" customFormat="1" ht="57.6">
+      <c r="A16" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="5">
-        <v>45923</v>
-      </c>
-      <c r="K16" s="9" t="s">
+      <c r="J16" s="19">
+        <v>45923</v>
+      </c>
+      <c r="K16" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="8">
+      <c r="L16" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="21">
         <v>1</v>
       </c>
     </row>
@@ -3235,10 +3285,10 @@
       <c r="K17" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="8">
+      <c r="L17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3276,10 +3326,10 @@
       <c r="K18" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" s="8">
+      <c r="L18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3317,10 +3367,10 @@
       <c r="K19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" s="8">
+      <c r="L19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3358,10 +3408,10 @@
       <c r="K20" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M20" s="8">
+      <c r="L20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3399,10 +3449,10 @@
       <c r="K21" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="8">
+      <c r="L21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3440,10 +3490,10 @@
       <c r="K22" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="8">
+      <c r="L22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3481,10 +3531,10 @@
       <c r="K23" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23" s="8">
+      <c r="L23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3522,10 +3572,10 @@
       <c r="K24" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" s="8">
+      <c r="L24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3563,10 +3613,10 @@
       <c r="K25" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="L25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="8">
+      <c r="L25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3604,10 +3654,10 @@
       <c r="K26" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26" s="8">
+      <c r="L26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3645,10 +3695,10 @@
       <c r="K27" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="L27" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M27" s="8">
+      <c r="L27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3686,10 +3736,10 @@
       <c r="K28" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="L28" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M28" s="8">
+      <c r="L28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3724,13 +3774,13 @@
       <c r="J29" s="5">
         <v>45923</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="L29" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29" s="8">
+      <c r="L29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3768,10 +3818,10 @@
       <c r="K30" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="L30" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30" s="8">
+      <c r="L30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3809,51 +3859,51 @@
       <c r="K31" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="L31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31" s="8">
+      <c r="L31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="28.8">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="9" t="s">
         <v>234</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="10">
         <v>45923</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="L32" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M32" s="8">
+      <c r="M32" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3882,7 +3932,7 @@
       <c r="H33" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I33" s="9" t="s">
         <v>241</v>
       </c>
       <c r="J33" s="5">
@@ -3891,10 +3941,10 @@
       <c r="K33" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="L33" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M33" s="8">
+      <c r="M33" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3923,7 +3973,7 @@
       <c r="H34" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="I34" s="11" t="s">
+      <c r="I34" s="9" t="s">
         <v>241</v>
       </c>
       <c r="J34" s="5">
@@ -3932,10 +3982,10 @@
       <c r="K34" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="L34" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M34" s="8">
+      <c r="M34" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3973,10 +4023,10 @@
       <c r="K35" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M35" s="8">
+      <c r="L35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4014,10 +4064,10 @@
       <c r="K36" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" s="8">
+      <c r="L36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4055,10 +4105,10 @@
       <c r="K37" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M37" s="8">
+      <c r="L37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4096,10 +4146,10 @@
       <c r="K38" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M38" s="8">
+      <c r="L38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4137,10 +4187,10 @@
       <c r="K39" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M39" s="8">
+      <c r="L39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4178,10 +4228,10 @@
       <c r="K40" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M40" s="8">
+      <c r="L40" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4219,10 +4269,10 @@
       <c r="K41" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M41" s="8">
+      <c r="L41" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M41" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4260,10 +4310,10 @@
       <c r="K42" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="L42" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M42" s="8">
+      <c r="L42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4301,10 +4351,10 @@
       <c r="K43" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="L43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M43" s="8">
+      <c r="L43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4333,7 +4383,7 @@
       <c r="H44" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="I44" s="9" t="s">
         <v>241</v>
       </c>
       <c r="J44" s="5">
@@ -4342,10 +4392,10 @@
       <c r="K44" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L44" s="13" t="s">
+      <c r="L44" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M44" s="8">
+      <c r="M44" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4383,10 +4433,10 @@
       <c r="K45" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M45" s="8">
+      <c r="L45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4424,10 +4474,10 @@
       <c r="K46" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="L46" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M46" s="8">
+      <c r="L46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M46" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4465,10 +4515,10 @@
       <c r="K47" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="L47" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M47" s="8">
+      <c r="L47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4506,10 +4556,10 @@
       <c r="K48" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="L48" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M48" s="8">
+      <c r="L48" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4547,10 +4597,10 @@
       <c r="K49" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L49" s="13" t="s">
+      <c r="L49" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M49" s="8">
+      <c r="M49" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4588,10 +4638,10 @@
       <c r="K50" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="L50" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M50" s="8">
+      <c r="L50" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M50" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4629,10 +4679,10 @@
       <c r="K51" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="L51" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M51" s="8">
+      <c r="L51" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M51" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4670,10 +4720,10 @@
       <c r="K52" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="L52" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M52" s="8">
+      <c r="L52" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M52" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4711,10 +4761,10 @@
       <c r="K53" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L53" s="13" t="s">
+      <c r="L53" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M53" s="8">
+      <c r="M53" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4752,10 +4802,10 @@
       <c r="K54" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L54" s="13" t="s">
+      <c r="L54" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M54" s="8">
+      <c r="M54" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4793,10 +4843,10 @@
       <c r="K55" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="L55" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M55" s="8">
+      <c r="L55" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M55" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4834,10 +4884,10 @@
       <c r="K56" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="L56" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M56" s="8">
+      <c r="L56" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M56" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4875,10 +4925,10 @@
       <c r="K57" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L57" s="13" t="s">
+      <c r="L57" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M57" s="8">
+      <c r="M57" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4916,10 +4966,10 @@
       <c r="K58" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="L58" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M58" s="8">
+      <c r="L58" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M58" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4957,10 +5007,10 @@
       <c r="K59" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L59" s="13" t="s">
+      <c r="L59" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M59" s="8">
+      <c r="M59" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4998,10 +5048,10 @@
       <c r="K60" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="L60" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M60" s="8">
+      <c r="L60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5039,10 +5089,10 @@
       <c r="K61" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="L61" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M61" s="8">
+      <c r="L61" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M61" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5080,10 +5130,10 @@
       <c r="K62" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="L62" s="13" t="s">
+      <c r="L62" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="M62" s="8">
+      <c r="M62" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5121,10 +5171,10 @@
       <c r="K63" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="L63" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M63" s="8">
+      <c r="L63" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M63" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5162,10 +5212,10 @@
       <c r="K64" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="L64" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M64" s="8">
+      <c r="L64" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M64" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5203,10 +5253,10 @@
       <c r="K65" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="L65" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M65" s="8">
+      <c r="L65" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M65" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5244,10 +5294,10 @@
       <c r="K66" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="L66" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M66" s="8">
+      <c r="L66" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M66" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5285,10 +5335,10 @@
       <c r="K67" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="L67" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M67" s="8">
+      <c r="L67" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M67" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5326,10 +5376,10 @@
       <c r="K68" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="L68" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M68" s="8">
+      <c r="L68" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5367,10 +5417,10 @@
       <c r="K69" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="L69" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M69" s="8">
+      <c r="L69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M69" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5408,10 +5458,10 @@
       <c r="K70" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="L70" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M70" s="8">
+      <c r="L70" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M70" s="7">
         <v>1</v>
       </c>
     </row>
@@ -5449,15 +5499,15 @@
       <c r="K71" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="L71" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M71" s="8">
+      <c r="L71" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M71" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:13">
-      <c r="M72" s="8"/>
+      <c r="M72" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>